<commit_message>
- Fix Tile's template and blockSize - Add Pause and Event Handling Note: Hold function is NOT implemented
</commit_message>
<xml_diff>
--- a/Prototype.xlsx
+++ b/Prototype.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -42,8 +42,14 @@
       <name val="TH SarabunPSK"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="TH SarabunPSK"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +128,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -150,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -177,8 +189,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -187,6 +205,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF52FF"/>
       <color rgb="FFFF8CFF"/>
       <color rgb="FFA552FF"/>
       <color rgb="FFFF7628"/>
@@ -463,15 +482,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD36"/>
+  <dimension ref="A1:AT36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AQ16" sqref="AQ16"/>
+      <selection activeCell="AO14" sqref="AO14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B1" s="10">
         <v>0</v>
       </c>
@@ -534,15 +553,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="13">
+      <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="3"/>
@@ -551,43 +570,46 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="2"/>
+      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="10">
         <v>0</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="2"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="10">
         <v>0</v>
       </c>
-      <c r="S2" s="1"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
       <c r="W2" s="10">
         <v>0</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="21"/>
       <c r="AB2" s="10">
         <v>0</v>
       </c>
-      <c r="AD2" s="18"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD2" s="19">
+        <v>3</v>
+      </c>
+      <c r="AO2" s="12"/>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="13">
+      <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3" s="3"/>
@@ -596,65 +618,66 @@
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="2"/>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="10">
         <v>1</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="2"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="10">
         <v>1</v>
       </c>
-      <c r="S3" s="1"/>
+      <c r="S3" s="2"/>
       <c r="T3" s="2"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
       <c r="W3" s="10">
         <v>1</v>
       </c>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
+      <c r="AA3" s="21"/>
       <c r="AB3" s="10">
         <v>1</v>
       </c>
-      <c r="AD3" s="18"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD3" s="19"/>
+      <c r="AO3" s="12"/>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="13">
+      <c r="E4" s="2"/>
+      <c r="F4" s="10">
         <v>2</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="10">
         <v>2</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="1"/>
+      <c r="L4" s="2"/>
       <c r="M4" s="10">
         <v>2</v>
       </c>
-      <c r="N4" s="2"/>
+      <c r="N4" s="21"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
       <c r="R4" s="10">
         <v>2</v>
       </c>
       <c r="S4" s="1"/>
-      <c r="T4" s="2"/>
+      <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="10">
@@ -662,44 +685,44 @@
       </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="21"/>
       <c r="AB4" s="10">
         <v>2</v>
       </c>
-      <c r="AD4" s="18"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD4" s="19"/>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="15">
+      <c r="F5" s="10">
         <v>3</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="10">
         <v>3</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="1"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
       <c r="M5" s="10">
         <v>3</v>
       </c>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="2"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="10">
         <v>3</v>
       </c>
       <c r="S5" s="1"/>
-      <c r="T5" s="2"/>
+      <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="10">
@@ -707,14 +730,14 @@
       </c>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="21"/>
       <c r="AB5" s="10">
         <v>3</v>
       </c>
-      <c r="AD5" s="18"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD5" s="19"/>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B6" s="10">
         <v>0</v>
       </c>
@@ -777,13 +800,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>0</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="11"/>
       <c r="F7" s="13">
         <v>0</v>
@@ -794,40 +817,42 @@
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="K7" s="4"/>
       <c r="L7" s="11"/>
       <c r="M7" s="13">
         <v>0</v>
       </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="1"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="4"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="13">
         <v>0</v>
       </c>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
       <c r="V7" s="11"/>
       <c r="W7" s="13">
         <v>0</v>
       </c>
-      <c r="X7" s="1"/>
+      <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
+      <c r="Z7" s="21"/>
       <c r="AA7" s="11"/>
       <c r="AB7" s="10">
         <v>0</v>
       </c>
-      <c r="AD7" s="19"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD7" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>1</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="11"/>
       <c r="F8" s="13">
@@ -837,43 +862,43 @@
       <c r="H8" s="13">
         <v>1</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="11"/>
       <c r="M8" s="13">
         <v>1</v>
       </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="1"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="4"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="11"/>
       <c r="R8" s="13">
         <v>1</v>
       </c>
       <c r="S8" s="4"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
       <c r="V8" s="11"/>
       <c r="W8" s="13">
         <v>1</v>
       </c>
       <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="21"/>
       <c r="AA8" s="11"/>
       <c r="AB8" s="10">
         <v>1</v>
       </c>
-      <c r="AD8" s="19"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD8" s="20"/>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>2</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="11"/>
       <c r="F9" s="13">
         <v>2</v>
@@ -882,21 +907,21 @@
       <c r="H9" s="13">
         <v>2</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
       <c r="L9" s="11"/>
       <c r="M9" s="13">
         <v>2</v>
       </c>
-      <c r="N9" s="4"/>
+      <c r="N9" s="21"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="1"/>
+      <c r="P9" s="4"/>
       <c r="Q9" s="11"/>
       <c r="R9" s="13">
         <v>2</v>
       </c>
-      <c r="S9" s="1"/>
+      <c r="S9" s="4"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="11"/>
@@ -904,15 +929,15 @@
         <v>2</v>
       </c>
       <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="21"/>
       <c r="AA9" s="11"/>
       <c r="AB9" s="10">
         <v>2</v>
       </c>
-      <c r="AD9" s="19"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD9" s="20"/>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>3</v>
       </c>
@@ -955,9 +980,13 @@
       <c r="AB10" s="10">
         <v>3</v>
       </c>
-      <c r="AD10" s="19"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD10" s="20"/>
+      <c r="AO10" s="18"/>
+      <c r="AR10" s="18"/>
+      <c r="AS10" s="18"/>
+      <c r="AT10" s="18"/>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B11" s="10">
         <v>0</v>
       </c>
@@ -1024,12 +1053,15 @@
       <c r="AA11" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD11" s="20"/>
+      <c r="AO11" s="18"/>
+      <c r="AT11" s="18"/>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>0</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="11"/>
@@ -1040,43 +1072,47 @@
       <c r="H12" s="13">
         <v>0</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="11"/>
       <c r="M12" s="13">
         <v>0</v>
       </c>
-      <c r="N12" s="5"/>
+      <c r="N12" s="21"/>
       <c r="O12" s="5"/>
-      <c r="P12" s="1"/>
+      <c r="P12" s="5"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="13">
         <v>0</v>
       </c>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
       <c r="V12" s="11"/>
       <c r="W12" s="13">
         <v>0</v>
       </c>
       <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="21"/>
       <c r="AA12" s="11"/>
       <c r="AB12" s="10">
         <v>0</v>
       </c>
-      <c r="AD12" s="19"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD12" s="20"/>
+      <c r="AO12" s="18"/>
+      <c r="AP12" s="18"/>
+      <c r="AS12" s="18"/>
+      <c r="AT12" s="18"/>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>1</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="11"/>
       <c r="F13" s="13">
         <v>1</v>
@@ -1086,42 +1122,48 @@
         <v>1</v>
       </c>
       <c r="I13" s="5"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
       <c r="L13" s="11"/>
       <c r="M13" s="13">
         <v>1</v>
       </c>
-      <c r="N13" s="5"/>
-      <c r="O13" s="1"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="5"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="13">
         <v>1</v>
       </c>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
       <c r="U13" s="5"/>
       <c r="V13" s="11"/>
       <c r="W13" s="13">
         <v>1</v>
       </c>
       <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="21"/>
       <c r="AA13" s="11"/>
       <c r="AB13" s="10">
         <v>1</v>
       </c>
-      <c r="AD13" s="19"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD13" s="20"/>
+      <c r="AO13" s="18"/>
+      <c r="AP13" s="18"/>
+      <c r="AQ13" s="18"/>
+      <c r="AR13" s="18"/>
+      <c r="AS13" s="18"/>
+      <c r="AT13" s="18"/>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>2</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="11"/>
       <c r="F14" s="13">
         <v>2</v>
@@ -1130,15 +1172,15 @@
       <c r="H14" s="13">
         <v>2</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
       <c r="L14" s="11"/>
       <c r="M14" s="13">
         <v>2</v>
       </c>
-      <c r="N14" s="5"/>
-      <c r="O14" s="1"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="5"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="13">
@@ -1146,21 +1188,21 @@
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
+      <c r="U14" s="5"/>
       <c r="V14" s="11"/>
       <c r="W14" s="13">
         <v>2</v>
       </c>
-      <c r="X14" s="1"/>
+      <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
+      <c r="Z14" s="21"/>
       <c r="AA14" s="11"/>
       <c r="AB14" s="10">
         <v>2</v>
       </c>
-      <c r="AD14" s="19"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AD14" s="20"/>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>3</v>
       </c>
@@ -1203,22 +1245,22 @@
       <c r="AB15" s="10">
         <v>3</v>
       </c>
-      <c r="AD15" s="19"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B16" s="10">
-        <v>0</v>
-      </c>
-      <c r="C16" s="10">
-        <v>1</v>
-      </c>
-      <c r="D16" s="10">
+      <c r="AD15" s="20"/>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="A16" s="14"/>
+      <c r="B16" s="13">
+        <v>0</v>
+      </c>
+      <c r="C16" s="13">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13">
         <v>2</v>
       </c>
       <c r="E16" s="10">
         <v>3</v>
       </c>
-      <c r="F16" s="12"/>
       <c r="G16" s="17"/>
       <c r="H16" s="14"/>
       <c r="I16" s="13">
@@ -1233,7 +1275,6 @@
       <c r="L16" s="10">
         <v>3</v>
       </c>
-      <c r="M16" s="14"/>
       <c r="N16" s="13">
         <v>0</v>
       </c>
@@ -1272,16 +1313,18 @@
       <c r="AA16" s="10">
         <v>3</v>
       </c>
+      <c r="AB16" s="14"/>
+      <c r="AD16" s="20"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A17" s="10">
+      <c r="A17" s="13">
         <v>0</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="6"/>
       <c r="D17" s="1"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="13">
+      <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="16"/>
@@ -1292,55 +1335,55 @@
       <c r="J17" s="6"/>
       <c r="K17" s="1"/>
       <c r="L17" s="11"/>
-      <c r="M17" s="13">
-        <v>0</v>
-      </c>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
+      <c r="M17" s="10">
+        <v>0</v>
+      </c>
+      <c r="N17" s="21"/>
+      <c r="O17" s="6"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="13">
         <v>0</v>
       </c>
-      <c r="S17" s="1"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="1"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
       <c r="V17" s="11"/>
       <c r="W17" s="13">
         <v>0</v>
       </c>
       <c r="X17" s="1"/>
       <c r="Y17" s="6"/>
-      <c r="Z17" s="1"/>
+      <c r="Z17" s="21"/>
       <c r="AA17" s="11"/>
-      <c r="AB17" s="10">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="19"/>
+      <c r="AB17" s="13">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="20"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A18" s="10">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1"/>
+      <c r="A18" s="13">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="13">
+      <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="13">
         <v>1</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="11"/>
-      <c r="M18" s="13">
-        <v>1</v>
-      </c>
-      <c r="N18" s="6"/>
+      <c r="M18" s="10">
+        <v>1</v>
+      </c>
+      <c r="N18" s="21"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="11"/>
@@ -1349,43 +1392,43 @@
       </c>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
-      <c r="U18" s="1"/>
+      <c r="U18" s="6"/>
       <c r="V18" s="11"/>
       <c r="W18" s="13">
         <v>1</v>
       </c>
       <c r="X18" s="6"/>
       <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
+      <c r="Z18" s="21"/>
       <c r="AA18" s="11"/>
-      <c r="AB18" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD18" s="19"/>
+      <c r="AB18" s="13">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="20"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
+      <c r="A19" s="13">
         <v>2</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="6"/>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="13">
+      <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="13">
         <v>2</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="1"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
       <c r="L19" s="11"/>
-      <c r="M19" s="13">
-        <v>2</v>
-      </c>
-      <c r="N19" s="1"/>
+      <c r="M19" s="10">
+        <v>2</v>
+      </c>
+      <c r="N19" s="21"/>
       <c r="O19" s="6"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="11"/>
@@ -1400,23 +1443,23 @@
         <v>2</v>
       </c>
       <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="21"/>
       <c r="AA19" s="11"/>
-      <c r="AB19" s="10">
-        <v>2</v>
-      </c>
-      <c r="AD19" s="19"/>
+      <c r="AB19" s="13">
+        <v>2</v>
+      </c>
+      <c r="AD19" s="20"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A20" s="10">
+      <c r="A20" s="15">
         <v>3</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="15">
+      <c r="F20" s="10">
         <v>3</v>
       </c>
       <c r="G20" s="17"/>
@@ -1427,7 +1470,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
-      <c r="M20" s="15">
+      <c r="M20" s="10">
         <v>3</v>
       </c>
       <c r="N20" s="11"/>
@@ -1448,10 +1491,10 @@
       <c r="Y20" s="11"/>
       <c r="Z20" s="11"/>
       <c r="AA20" s="11"/>
-      <c r="AB20" s="10">
-        <v>3</v>
-      </c>
-      <c r="AD20" s="19"/>
+      <c r="AB20" s="15">
+        <v>3</v>
+      </c>
+      <c r="AD20" s="20"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B21" s="10">
@@ -1468,20 +1511,19 @@
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="17"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="13">
-        <v>0</v>
-      </c>
-      <c r="J21" s="13">
-        <v>1</v>
-      </c>
-      <c r="K21" s="13">
+      <c r="I21" s="10">
+        <v>0</v>
+      </c>
+      <c r="J21" s="10">
+        <v>1</v>
+      </c>
+      <c r="K21" s="10">
         <v>2</v>
       </c>
       <c r="L21" s="10">
         <v>3</v>
       </c>
-      <c r="M21" s="14"/>
+      <c r="M21" s="12"/>
       <c r="N21" s="13">
         <v>0</v>
       </c>
@@ -1522,12 +1564,12 @@
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22" s="10">
-        <v>0</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="A22" s="13">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
       <c r="E22" s="11"/>
       <c r="F22" s="13">
         <v>0</v>
@@ -1536,38 +1578,40 @@
       <c r="H22" s="13">
         <v>0</v>
       </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
       <c r="L22" s="11"/>
       <c r="M22" s="13">
         <v>0</v>
       </c>
-      <c r="N22" s="1"/>
+      <c r="N22" s="21"/>
       <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
+      <c r="P22" s="1"/>
       <c r="Q22" s="11"/>
       <c r="R22" s="13">
         <v>0</v>
       </c>
-      <c r="S22" s="1"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="1"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
       <c r="V22" s="11"/>
-      <c r="W22" s="13">
-        <v>0</v>
-      </c>
-      <c r="X22" s="1"/>
+      <c r="W22" s="10">
+        <v>0</v>
+      </c>
+      <c r="X22" s="8"/>
       <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
+      <c r="Z22" s="21"/>
       <c r="AA22" s="11"/>
-      <c r="AB22" s="10">
-        <v>0</v>
-      </c>
-      <c r="AD22" s="18"/>
+      <c r="AB22" s="13">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="19">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A23" s="10">
+      <c r="A23" s="13">
         <v>1</v>
       </c>
       <c r="B23" s="8"/>
@@ -1588,9 +1632,9 @@
       <c r="M23" s="13">
         <v>1</v>
       </c>
-      <c r="N23" s="8"/>
+      <c r="N23" s="21"/>
       <c r="O23" s="8"/>
-      <c r="P23" s="1"/>
+      <c r="P23" s="8"/>
       <c r="Q23" s="11"/>
       <c r="R23" s="13">
         <v>1</v>
@@ -1599,24 +1643,24 @@
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
       <c r="V23" s="11"/>
-      <c r="W23" s="13">
-        <v>1</v>
-      </c>
-      <c r="X23" s="1"/>
+      <c r="W23" s="10">
+        <v>1</v>
+      </c>
+      <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
-      <c r="Z23" s="8"/>
+      <c r="Z23" s="21"/>
       <c r="AA23" s="11"/>
-      <c r="AB23" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD23" s="18"/>
+      <c r="AB23" s="13">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="19"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24" s="10">
+      <c r="A24" s="13">
         <v>2</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="8"/>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="11"/>
       <c r="F24" s="13">
@@ -1626,38 +1670,38 @@
       <c r="H24" s="13">
         <v>2</v>
       </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="1"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
       <c r="L24" s="11"/>
       <c r="M24" s="13">
         <v>2</v>
       </c>
-      <c r="N24" s="1"/>
+      <c r="N24" s="21"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
+      <c r="P24" s="8"/>
       <c r="Q24" s="11"/>
       <c r="R24" s="13">
         <v>2</v>
       </c>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="1"/>
       <c r="V24" s="11"/>
-      <c r="W24" s="13">
-        <v>2</v>
-      </c>
-      <c r="X24" s="8"/>
+      <c r="W24" s="10">
+        <v>2</v>
+      </c>
+      <c r="X24" s="1"/>
       <c r="Y24" s="8"/>
-      <c r="Z24" s="1"/>
+      <c r="Z24" s="21"/>
       <c r="AA24" s="11"/>
-      <c r="AB24" s="10">
-        <v>2</v>
-      </c>
-      <c r="AD24" s="18"/>
+      <c r="AB24" s="13">
+        <v>2</v>
+      </c>
+      <c r="AD24" s="19"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A25" s="10">
+      <c r="A25" s="15">
         <v>3</v>
       </c>
       <c r="B25" s="11"/>
@@ -1689,17 +1733,17 @@
       <c r="T25" s="11"/>
       <c r="U25" s="11"/>
       <c r="V25" s="11"/>
-      <c r="W25" s="15">
+      <c r="W25" s="10">
         <v>3</v>
       </c>
       <c r="X25" s="11"/>
       <c r="Y25" s="11"/>
       <c r="Z25" s="11"/>
       <c r="AA25" s="11"/>
-      <c r="AB25" s="10">
-        <v>3</v>
-      </c>
-      <c r="AD25" s="18"/>
+      <c r="AB25" s="15">
+        <v>3</v>
+      </c>
+      <c r="AD25" s="19"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B26" s="10">
@@ -1716,14 +1760,13 @@
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="17"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="13">
-        <v>0</v>
-      </c>
-      <c r="J26" s="13">
-        <v>1</v>
-      </c>
-      <c r="K26" s="13">
+      <c r="I26" s="10">
+        <v>0</v>
+      </c>
+      <c r="J26" s="10">
+        <v>1</v>
+      </c>
+      <c r="K26" s="10">
         <v>2</v>
       </c>
       <c r="L26" s="10">
@@ -1768,61 +1811,63 @@
       <c r="AA26" s="10">
         <v>3</v>
       </c>
+      <c r="AB26" s="12"/>
+      <c r="AD26" s="19"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A27" s="10">
-        <v>0</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="9"/>
+      <c r="A27" s="13">
+        <v>0</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="1"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="13">
+      <c r="F27" s="10">
         <v>0</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="13">
         <v>0</v>
       </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="1"/>
       <c r="L27" s="11"/>
       <c r="M27" s="13">
         <v>0</v>
       </c>
-      <c r="N27" s="1"/>
+      <c r="N27" s="21"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
+      <c r="P27" s="9"/>
       <c r="Q27" s="11"/>
       <c r="R27" s="13">
         <v>0</v>
       </c>
-      <c r="S27" s="1"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="1"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21"/>
+      <c r="U27" s="21"/>
       <c r="V27" s="11"/>
       <c r="W27" s="13">
         <v>0</v>
       </c>
-      <c r="X27" s="9"/>
+      <c r="X27" s="1"/>
       <c r="Y27" s="9"/>
-      <c r="Z27" s="1"/>
+      <c r="Z27" s="21"/>
       <c r="AA27" s="11"/>
       <c r="AB27" s="10">
         <v>0</v>
       </c>
-      <c r="AD27" s="18"/>
+      <c r="AD27" s="19"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A28" s="10">
+      <c r="A28" s="13">
         <v>1</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="11"/>
-      <c r="F28" s="13">
+      <c r="F28" s="10">
         <v>1</v>
       </c>
       <c r="G28" s="16"/>
@@ -1836,9 +1881,9 @@
       <c r="M28" s="13">
         <v>1</v>
       </c>
-      <c r="N28" s="9"/>
+      <c r="N28" s="21"/>
       <c r="O28" s="9"/>
-      <c r="P28" s="1"/>
+      <c r="P28" s="9"/>
       <c r="Q28" s="11"/>
       <c r="R28" s="13">
         <v>1</v>
@@ -1850,69 +1895,69 @@
       <c r="W28" s="13">
         <v>1</v>
       </c>
-      <c r="X28" s="1"/>
+      <c r="X28" s="9"/>
       <c r="Y28" s="9"/>
-      <c r="Z28" s="9"/>
+      <c r="Z28" s="21"/>
       <c r="AA28" s="11"/>
       <c r="AB28" s="10">
         <v>1</v>
       </c>
-      <c r="AD28" s="18"/>
+      <c r="AD28" s="19"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A29" s="10">
+      <c r="A29" s="13">
         <v>2</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="9"/>
+      <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="11"/>
-      <c r="F29" s="13">
+      <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="13">
         <v>2</v>
       </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="1"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
       <c r="L29" s="11"/>
       <c r="M29" s="13">
         <v>2</v>
       </c>
-      <c r="N29" s="1"/>
+      <c r="N29" s="21"/>
       <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
+      <c r="P29" s="1"/>
       <c r="Q29" s="11"/>
       <c r="R29" s="13">
         <v>2</v>
       </c>
-      <c r="S29" s="9"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
       <c r="V29" s="11"/>
       <c r="W29" s="13">
         <v>2</v>
       </c>
-      <c r="X29" s="1"/>
+      <c r="X29" s="9"/>
       <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
+      <c r="Z29" s="21"/>
       <c r="AA29" s="11"/>
       <c r="AB29" s="10">
         <v>2</v>
       </c>
-      <c r="AD29" s="18"/>
+      <c r="AD29" s="19"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A30" s="10">
+      <c r="A30" s="15">
         <v>3</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
-      <c r="F30" s="15">
+      <c r="F30" s="10">
         <v>3</v>
       </c>
       <c r="G30" s="3"/>
@@ -1947,7 +1992,7 @@
       <c r="AB30" s="10">
         <v>3</v>
       </c>
-      <c r="AD30" s="18"/>
+      <c r="AD30" s="19"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B31" s="10">
@@ -2055,7 +2100,9 @@
       <c r="AB32" s="10">
         <v>0</v>
       </c>
-      <c r="AD32" s="19"/>
+      <c r="AD32" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
@@ -2100,7 +2147,7 @@
       <c r="AB33" s="10">
         <v>1</v>
       </c>
-      <c r="AD33" s="19"/>
+      <c r="AD33" s="20"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
@@ -2145,7 +2192,7 @@
       <c r="AB34" s="10">
         <v>2</v>
       </c>
-      <c r="AD34" s="19"/>
+      <c r="AD34" s="20"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="10">
@@ -2190,7 +2237,7 @@
       <c r="AB35" s="10">
         <v>3</v>
       </c>
-      <c r="AD35" s="19"/>
+      <c r="AD35" s="20"/>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B36" s="10">
@@ -2256,6 +2303,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="AD2:AD5"/>
+    <mergeCell ref="AD7:AD20"/>
+    <mergeCell ref="AD22:AD30"/>
+    <mergeCell ref="AD32:AD35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes: turnClockwise and lineClear
</commit_message>
<xml_diff>
--- a/Prototype.xlsx
+++ b/Prototype.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -162,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -189,14 +189,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +484,7 @@
   <dimension ref="A1:AT36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO14" sqref="AO14"/>
+      <selection activeCell="AM8" sqref="AM8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,24 +574,24 @@
       <c r="M2" s="10">
         <v>0</v>
       </c>
-      <c r="N2" s="21"/>
+      <c r="N2" s="18"/>
       <c r="O2" s="2"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="10">
         <v>0</v>
       </c>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
       <c r="W2" s="10">
         <v>0</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="2"/>
-      <c r="AA2" s="21"/>
+      <c r="AA2" s="18"/>
       <c r="AB2" s="10">
         <v>0</v>
       </c>
@@ -623,7 +622,7 @@
       <c r="M3" s="10">
         <v>1</v>
       </c>
-      <c r="N3" s="21"/>
+      <c r="N3" s="18"/>
       <c r="O3" s="2"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -640,7 +639,7 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="21"/>
+      <c r="AA3" s="18"/>
       <c r="AB3" s="10">
         <v>1</v>
       </c>
@@ -669,7 +668,7 @@
       <c r="M4" s="10">
         <v>2</v>
       </c>
-      <c r="N4" s="21"/>
+      <c r="N4" s="18"/>
       <c r="O4" s="2"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -686,7 +685,7 @@
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="2"/>
-      <c r="AA4" s="21"/>
+      <c r="AA4" s="18"/>
       <c r="AB4" s="10">
         <v>2</v>
       </c>
@@ -707,14 +706,14 @@
       <c r="H5" s="10">
         <v>3</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
       <c r="M5" s="10">
         <v>3</v>
       </c>
-      <c r="N5" s="21"/>
+      <c r="N5" s="18"/>
       <c r="O5" s="2"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -731,7 +730,7 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="2"/>
-      <c r="AA5" s="21"/>
+      <c r="AA5" s="18"/>
       <c r="AB5" s="10">
         <v>3</v>
       </c>
@@ -822,23 +821,23 @@
       <c r="M7" s="13">
         <v>0</v>
       </c>
-      <c r="N7" s="21"/>
+      <c r="N7" s="18"/>
       <c r="O7" s="4"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="13">
         <v>0</v>
       </c>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
       <c r="V7" s="11"/>
       <c r="W7" s="13">
         <v>0</v>
       </c>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
-      <c r="Z7" s="21"/>
+      <c r="Z7" s="18"/>
       <c r="AA7" s="11"/>
       <c r="AB7" s="10">
         <v>0</v>
@@ -869,7 +868,7 @@
       <c r="M8" s="13">
         <v>1</v>
       </c>
-      <c r="N8" s="21"/>
+      <c r="N8" s="18"/>
       <c r="O8" s="4"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="11"/>
@@ -885,7 +884,7 @@
       </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="4"/>
-      <c r="Z8" s="21"/>
+      <c r="Z8" s="18"/>
       <c r="AA8" s="11"/>
       <c r="AB8" s="10">
         <v>1</v>
@@ -907,14 +906,14 @@
       <c r="H9" s="13">
         <v>2</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
       <c r="L9" s="11"/>
       <c r="M9" s="13">
         <v>2</v>
       </c>
-      <c r="N9" s="21"/>
+      <c r="N9" s="18"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="11"/>
@@ -930,7 +929,7 @@
       </c>
       <c r="X9" s="1"/>
       <c r="Y9" s="4"/>
-      <c r="Z9" s="21"/>
+      <c r="Z9" s="18"/>
       <c r="AA9" s="11"/>
       <c r="AB9" s="10">
         <v>2</v>
@@ -981,10 +980,13 @@
         <v>3</v>
       </c>
       <c r="AD10" s="20"/>
-      <c r="AO10" s="18"/>
-      <c r="AR10" s="18"/>
-      <c r="AS10" s="18"/>
-      <c r="AT10" s="18"/>
+      <c r="AN10" s="12"/>
+      <c r="AO10" s="12"/>
+      <c r="AP10" s="12"/>
+      <c r="AQ10" s="12"/>
+      <c r="AR10" s="12"/>
+      <c r="AS10" s="12"/>
+      <c r="AT10" s="12"/>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B11" s="10">
@@ -1054,8 +1056,13 @@
         <v>3</v>
       </c>
       <c r="AD11" s="20"/>
-      <c r="AO11" s="18"/>
-      <c r="AT11" s="18"/>
+      <c r="AN11" s="12"/>
+      <c r="AO11" s="12"/>
+      <c r="AP11" s="12"/>
+      <c r="AQ11" s="12"/>
+      <c r="AR11" s="12"/>
+      <c r="AS11" s="12"/>
+      <c r="AT11" s="12"/>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
@@ -1079,32 +1086,35 @@
       <c r="M12" s="13">
         <v>0</v>
       </c>
-      <c r="N12" s="21"/>
+      <c r="N12" s="18"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="13">
         <v>0</v>
       </c>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
+      <c r="U12" s="18"/>
       <c r="V12" s="11"/>
       <c r="W12" s="13">
         <v>0</v>
       </c>
       <c r="X12" s="1"/>
       <c r="Y12" s="5"/>
-      <c r="Z12" s="21"/>
+      <c r="Z12" s="18"/>
       <c r="AA12" s="11"/>
       <c r="AB12" s="10">
         <v>0</v>
       </c>
       <c r="AD12" s="20"/>
-      <c r="AO12" s="18"/>
-      <c r="AP12" s="18"/>
-      <c r="AS12" s="18"/>
-      <c r="AT12" s="18"/>
+      <c r="AN12" s="12"/>
+      <c r="AO12" s="12"/>
+      <c r="AP12" s="12"/>
+      <c r="AQ12" s="12"/>
+      <c r="AR12" s="12"/>
+      <c r="AS12" s="12"/>
+      <c r="AT12" s="12"/>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
@@ -1128,7 +1138,7 @@
       <c r="M13" s="13">
         <v>1</v>
       </c>
-      <c r="N13" s="21"/>
+      <c r="N13" s="18"/>
       <c r="O13" s="5"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="11"/>
@@ -1144,18 +1154,19 @@
       </c>
       <c r="X13" s="1"/>
       <c r="Y13" s="5"/>
-      <c r="Z13" s="21"/>
+      <c r="Z13" s="18"/>
       <c r="AA13" s="11"/>
       <c r="AB13" s="10">
         <v>1</v>
       </c>
       <c r="AD13" s="20"/>
-      <c r="AO13" s="18"/>
-      <c r="AP13" s="18"/>
-      <c r="AQ13" s="18"/>
-      <c r="AR13" s="18"/>
-      <c r="AS13" s="18"/>
-      <c r="AT13" s="18"/>
+      <c r="AN13" s="12"/>
+      <c r="AO13" s="12"/>
+      <c r="AP13" s="12"/>
+      <c r="AQ13" s="12"/>
+      <c r="AR13" s="12"/>
+      <c r="AS13" s="12"/>
+      <c r="AT13" s="12"/>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
@@ -1172,14 +1183,14 @@
       <c r="H14" s="13">
         <v>2</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
       <c r="L14" s="11"/>
       <c r="M14" s="13">
         <v>2</v>
       </c>
-      <c r="N14" s="21"/>
+      <c r="N14" s="18"/>
       <c r="O14" s="5"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="11"/>
@@ -1195,7 +1206,7 @@
       </c>
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
-      <c r="Z14" s="21"/>
+      <c r="Z14" s="18"/>
       <c r="AA14" s="11"/>
       <c r="AB14" s="10">
         <v>2</v>
@@ -1338,23 +1349,23 @@
       <c r="M17" s="10">
         <v>0</v>
       </c>
-      <c r="N17" s="21"/>
+      <c r="N17" s="18"/>
       <c r="O17" s="6"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="13">
         <v>0</v>
       </c>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="18"/>
       <c r="V17" s="11"/>
       <c r="W17" s="13">
         <v>0</v>
       </c>
       <c r="X17" s="1"/>
       <c r="Y17" s="6"/>
-      <c r="Z17" s="21"/>
+      <c r="Z17" s="18"/>
       <c r="AA17" s="11"/>
       <c r="AB17" s="13">
         <v>0</v>
@@ -1383,7 +1394,7 @@
       <c r="M18" s="10">
         <v>1</v>
       </c>
-      <c r="N18" s="21"/>
+      <c r="N18" s="18"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="11"/>
@@ -1399,7 +1410,7 @@
       </c>
       <c r="X18" s="6"/>
       <c r="Y18" s="6"/>
-      <c r="Z18" s="21"/>
+      <c r="Z18" s="18"/>
       <c r="AA18" s="11"/>
       <c r="AB18" s="13">
         <v>1</v>
@@ -1421,14 +1432,14 @@
       <c r="H19" s="13">
         <v>2</v>
       </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
       <c r="L19" s="11"/>
       <c r="M19" s="10">
         <v>2</v>
       </c>
-      <c r="N19" s="21"/>
+      <c r="N19" s="18"/>
       <c r="O19" s="6"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="11"/>
@@ -1444,7 +1455,7 @@
       </c>
       <c r="X19" s="1"/>
       <c r="Y19" s="6"/>
-      <c r="Z19" s="21"/>
+      <c r="Z19" s="18"/>
       <c r="AA19" s="11"/>
       <c r="AB19" s="13">
         <v>2</v>
@@ -1585,23 +1596,23 @@
       <c r="M22" s="13">
         <v>0</v>
       </c>
-      <c r="N22" s="21"/>
+      <c r="N22" s="18"/>
       <c r="O22" s="8"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="11"/>
       <c r="R22" s="13">
         <v>0</v>
       </c>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
+      <c r="U22" s="18"/>
       <c r="V22" s="11"/>
       <c r="W22" s="10">
         <v>0</v>
       </c>
       <c r="X22" s="8"/>
       <c r="Y22" s="1"/>
-      <c r="Z22" s="21"/>
+      <c r="Z22" s="18"/>
       <c r="AA22" s="11"/>
       <c r="AB22" s="13">
         <v>0</v>
@@ -1632,7 +1643,7 @@
       <c r="M23" s="13">
         <v>1</v>
       </c>
-      <c r="N23" s="21"/>
+      <c r="N23" s="18"/>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="11"/>
@@ -1648,7 +1659,7 @@
       </c>
       <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
-      <c r="Z23" s="21"/>
+      <c r="Z23" s="18"/>
       <c r="AA23" s="11"/>
       <c r="AB23" s="13">
         <v>1</v>
@@ -1670,14 +1681,14 @@
       <c r="H24" s="13">
         <v>2</v>
       </c>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
       <c r="L24" s="11"/>
       <c r="M24" s="13">
         <v>2</v>
       </c>
-      <c r="N24" s="21"/>
+      <c r="N24" s="18"/>
       <c r="O24" s="1"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="11"/>
@@ -1693,7 +1704,7 @@
       </c>
       <c r="X24" s="1"/>
       <c r="Y24" s="8"/>
-      <c r="Z24" s="21"/>
+      <c r="Z24" s="18"/>
       <c r="AA24" s="11"/>
       <c r="AB24" s="13">
         <v>2</v>
@@ -1836,23 +1847,23 @@
       <c r="M27" s="13">
         <v>0</v>
       </c>
-      <c r="N27" s="21"/>
+      <c r="N27" s="18"/>
       <c r="O27" s="1"/>
       <c r="P27" s="9"/>
       <c r="Q27" s="11"/>
       <c r="R27" s="13">
         <v>0</v>
       </c>
-      <c r="S27" s="21"/>
-      <c r="T27" s="21"/>
-      <c r="U27" s="21"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="18"/>
       <c r="V27" s="11"/>
       <c r="W27" s="13">
         <v>0</v>
       </c>
       <c r="X27" s="1"/>
       <c r="Y27" s="9"/>
-      <c r="Z27" s="21"/>
+      <c r="Z27" s="18"/>
       <c r="AA27" s="11"/>
       <c r="AB27" s="10">
         <v>0</v>
@@ -1881,7 +1892,7 @@
       <c r="M28" s="13">
         <v>1</v>
       </c>
-      <c r="N28" s="21"/>
+      <c r="N28" s="18"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
       <c r="Q28" s="11"/>
@@ -1897,7 +1908,7 @@
       </c>
       <c r="X28" s="9"/>
       <c r="Y28" s="9"/>
-      <c r="Z28" s="21"/>
+      <c r="Z28" s="18"/>
       <c r="AA28" s="11"/>
       <c r="AB28" s="10">
         <v>1</v>
@@ -1919,14 +1930,14 @@
       <c r="H29" s="13">
         <v>2</v>
       </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
       <c r="L29" s="11"/>
       <c r="M29" s="13">
         <v>2</v>
       </c>
-      <c r="N29" s="21"/>
+      <c r="N29" s="18"/>
       <c r="O29" s="9"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="11"/>
@@ -1942,7 +1953,7 @@
       </c>
       <c r="X29" s="9"/>
       <c r="Y29" s="1"/>
-      <c r="Z29" s="21"/>
+      <c r="Z29" s="18"/>
       <c r="AA29" s="11"/>
       <c r="AB29" s="10">
         <v>2</v>

</xml_diff>

<commit_message>
Line Number bug fixed and Clear Effect added
</commit_message>
<xml_diff>
--- a/Prototype.xlsx
+++ b/Prototype.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,7 +484,7 @@
   <dimension ref="A1:AT36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM8" sqref="AM8"/>
+      <selection activeCell="AE1" sqref="AE1:AU36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>